<commit_message>
[json] - [`addOrReplace(json,jsonpath,input,var)`](../commands/json(addOrReplace(json,jsonpath,input,var)): now supports   `json` either as JSON content or JSON file (must be fully qualified).
[web]
- [`executeScript(var,script)`](../commands/web/executeScript(var,script)): now support execution of
  JavaScript file.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_json.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_json.data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11206"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/ep/sentry/sentry-core/src/test/resources/showcase/artifact/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9153A611-38B7-DC40-8E24-43AFADAC374F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView tabRatio="500" windowHeight="12540" windowWidth="40960" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="440"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="10520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="#default" r:id="rId1" sheetId="2"/>
-    <sheet name="bad_jsonpath" r:id="rId2" sheetId="3"/>
+    <sheet name="#default" sheetId="2" r:id="rId1"/>
+    <sheet name="bad_jsonpath" sheetId="3" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -36,7 +37,7 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -49,36 +50,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>true</t>
   </si>
   <si>
-    <t>sentry.pollWaitMs</t>
-  </si>
-  <si>
-    <t>sentry.textDelim</t>
-  </si>
-  <si>
     <t>,</t>
   </si>
   <si>
-    <t>sentry.scope.iteration</t>
-  </si>
-  <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>sentry.scope.fallbackToPrevious</t>
-  </si>
-  <si>
-    <t>sentry.delayBetweenStepsMs</t>
-  </si>
-  <si>
-    <t>sentry.failFast</t>
-  </si>
-  <si>
-    <t>sentry.verbose</t>
   </si>
   <si>
     <t>false</t>
@@ -139,7 +119,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="7">
     <font>
       <sz val="12"/>
@@ -220,47 +199,47 @@
     </border>
   </borders>
   <cellStyleXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf applyFont="1" applyProtection="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="2"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="4"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="6"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="3"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="5"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -394,7 +373,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -413,7 +392,7 @@
       <sheetName val="#system"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData refreshError="1" sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -424,10 +403,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -462,7 +441,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -497,7 +476,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -591,21 +570,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -622,7 +601,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -674,32 +653,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAB10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AAA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="34.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="27.0" collapsed="true"/>
-    <col min="3" max="9" customWidth="true" style="3" width="27.0" collapsed="true"/>
-    <col min="10" max="27" customWidth="true" style="3" width="21.1640625" collapsed="true"/>
-    <col min="28" max="16384" style="3" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="34" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -709,60 +688,60 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
@@ -780,84 +759,84 @@
       <c r="AAA10" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection deleteColumns="0" deleteRows="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0"/>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule dxfId="9" operator="beginsWith" priority="1" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="9" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="8" operator="beginsWith" priority="2" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="8" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="7" priority="3" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule dxfId="6" priority="4" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="5" priority="5" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BB9477-0F10-0A45-A8BC-4B64FAFB9FBB}">
-  <dimension ref="A1:AAB10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BB9477-0F10-0A45-A8BC-4B64FAFB9FBB}">
+  <dimension ref="A1:AAA10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="144" zoomScaleNormal="125" zoomScalePageLayoutView="125">
+    <sheetView zoomScale="144" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="34.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="27.0" collapsed="true"/>
-    <col min="3" max="9" customWidth="true" style="3" width="27.0" collapsed="true"/>
-    <col min="10" max="27" customWidth="true" style="3" width="21.1640625" collapsed="true"/>
-    <col min="28" max="16384" style="3" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="34" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
@@ -887,27 +866,27 @@
       <c r="AAA10" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection deleteColumns="0" deleteRows="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0"/>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule dxfId="4" operator="beginsWith" priority="1" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="3" operator="beginsWith" priority="2" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="2" priority="3" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule dxfId="1" priority="4" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="0" priority="5" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>